<commit_message>
Dev From Office - added few read_it - added inteli msg - added readr auto mode - mark cell-analysis for remodeling into state - compatibility of cell traceback with external operations (like unpivotr etc) - added test Article (FileTypes) - added expore_it and other functions - read_it, read_tables (concept finalized) - multi routes tests - introduce grammer - todo %<^% kind of symbols for NNE etc - No merge to stable before next version
</commit_message>
<xml_diff>
--- a/00_nightly_only/whole_flow.xlsx
+++ b/00_nightly_only/whole_flow.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="74">
   <si>
     <t>function</t>
   </si>
@@ -125,12 +125,6 @@
     <t>Table_List</t>
   </si>
   <si>
-    <t>as_tcf</t>
-  </si>
-  <si>
-    <t>same as 'exploration_findings (with content)' &gt; as_tcf &gt; read.it</t>
-  </si>
-  <si>
     <t>complete heuristic based structure assignment (or partial operations)</t>
   </si>
   <si>
@@ -246,13 +240,19 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>as_tfc</t>
+  </si>
+  <si>
+    <t>same as 'exploration_findings (with content)' &gt; as_tfc &gt; read.it</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,6 +263,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Century Schoolbook"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Century Schoolbook"/>
       <family val="1"/>
     </font>
@@ -314,11 +320,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,7 +610,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -617,7 +625,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -634,7 +642,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -650,7 +658,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
@@ -665,7 +675,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
@@ -680,7 +692,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -700,7 +714,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>14</v>
@@ -715,7 +729,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>15</v>
@@ -724,19 +738,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3" t="s">
+    <row r="8" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>34</v>
+      <c r="E8" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -781,7 +795,7 @@
         <v>22</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -796,7 +810,7 @@
         <v>31</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -811,7 +825,7 @@
         <v>31</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -826,7 +840,7 @@
         <v>31</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -841,7 +855,7 @@
         <v>28</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -856,7 +870,7 @@
         <v>29</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -871,7 +885,7 @@
         <v>32</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -880,13 +894,13 @@
         <v>32</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -895,13 +909,13 @@
         <v>22</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -910,13 +924,13 @@
         <v>28</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -931,157 +945,157 @@
         <v>32</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="E22" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="E23" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="E24" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="E25" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="D26" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="E29" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dev V2 - Need to finish it quick - merge from home dev - readr auto mode may need fix - mark cell-analysis for remodeling into state - compatibility of cell traceback with external operations (like unpivotr etc) - added test Article (FileTypes) - multi routes tests - introduce grammer - todo %<^% kind of symbols for NNE etc - No merge to stable before next version
</commit_message>
<xml_diff>
--- a/00_nightly_only/whole_flow.xlsx
+++ b/00_nightly_only/whole_flow.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igayen\Documents\RBI\WorkSpace\R_Packages\Nightly\tidycells_nightly\00_nightly_only\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PenD\tidycells_nightly\00_nightly_only\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="76">
   <si>
     <t>function</t>
   </si>
@@ -246,6 +246,12 @@
   </si>
   <si>
     <t>same as 'exploration_findings (with content)' &gt; as_tfc &gt; read.it</t>
+  </si>
+  <si>
+    <t>reads meta (content info)</t>
+  </si>
+  <si>
+    <t>reads all tf contents and measures variations across TFs</t>
   </si>
 </sst>
 </file>
@@ -607,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -709,7 +715,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
@@ -724,7 +732,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
@@ -739,7 +749,9 @@
       </c>
     </row>
     <row r="8" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
+      <c r="A8" s="4">
+        <v>0</v>
+      </c>
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
@@ -753,8 +765,10 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
+    <row r="9" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
@@ -762,55 +776,61 @@
         <v>7</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>0</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E10" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -819,13 +839,13 @@
         <v>24</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -834,79 +854,79 @@
         <v>24</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E18" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>72</v>
@@ -915,13 +935,13 @@
         <v>15</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>72</v>
@@ -936,31 +956,31 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -969,13 +989,13 @@
         <v>42</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -984,13 +1004,13 @@
         <v>42</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -999,43 +1019,43 @@
         <v>42</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="E26" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="E27" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1044,13 +1064,13 @@
         <v>45</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>63</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1059,34 +1079,34 @@
         <v>45</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>65</v>
@@ -1095,6 +1115,21 @@
         <v>56</v>
       </c>
       <c r="E31" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Dev V2 - Need to finish it quick - mutate on cell-df introduced - working on corner block detection - read_cells / complete huristic detection can also be made like Table_List - mark cell-analysis for remodeling into state - compatibility of cell traceback with external operations (like unpivotr etc) - added test Article (FileTypes) - multi routes tests - introduce grammer - todo %<^% kind of symbols for NNE etc - No merge to stable before next version
</commit_message>
<xml_diff>
--- a/00_nightly_only/whole_flow.xlsx
+++ b/00_nightly_only/whole_flow.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PenD\tidycells_nightly\00_nightly_only\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igayen\Documents\RBI\WorkSpace\R_Packages\Nightly\tidycells_nightly\00_nightly_only\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="76">
   <si>
     <t>function</t>
   </si>
@@ -224,9 +224,6 @@
     <t>collate_columns</t>
   </si>
   <si>
-    <t>list (of data.frames)</t>
-  </si>
-  <si>
     <t>similar to rbind / bind_rows but with content based column collation (this is for standalonce use)</t>
   </si>
   <si>
@@ -252,6 +249,9 @@
   </si>
   <si>
     <t>reads all tf contents and measures variations across TFs</t>
+  </si>
+  <si>
+    <t>list (of data.frames) / Table_List</t>
   </si>
 </sst>
 </file>
@@ -616,7 +616,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -631,7 +631,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -648,7 +648,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -665,7 +665,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -682,7 +682,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
@@ -699,7 +699,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>8</v>
@@ -716,13 +716,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>14</v>
@@ -733,13 +733,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>15</v>
@@ -762,12 +762,12 @@
         <v>18</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>15</v>
@@ -776,10 +776,10 @@
         <v>7</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -801,7 +801,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>15</v>
@@ -818,7 +818,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>15</v>
@@ -875,11 +875,13 @@
         <v>31</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
+      <c r="A16" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="B16" s="3" t="s">
         <v>22</v>
       </c>
@@ -894,7 +896,9 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
+      <c r="A17" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
@@ -929,7 +933,7 @@
         <v>32</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>15</v>
@@ -944,7 +948,7 @@
         <v>22</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>15</v>
@@ -959,7 +963,7 @@
         <v>28</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>15</v>
@@ -1115,13 +1119,13 @@
         <v>56</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>65</v>
@@ -1130,7 +1134,7 @@
         <v>56</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dev V3 - Need to finish it quick - compatibility of cell traceback with external operations (like unpivotr etc) done - read_cells / complete huristic detection can also be made like Table_List - mark cell-analysis for remodeling into state (may be in laster version) - added test Article (FileTypes) - multi routes tests - introduce grammer - todo %<^% kind of symbols for NNE etc - No merge to stable before next version
</commit_message>
<xml_diff>
--- a/00_nightly_only/whole_flow.xlsx
+++ b/00_nightly_only/whole_flow.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="78">
   <si>
     <t>function</t>
   </si>
@@ -624,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1123,48 +1123,54 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3" t="s">
+    <row r="30" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3" t="s">
+    <row r="31" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3" t="s">
+    <row r="32" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="4" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>